<commit_message>
Add initial test files, configuration updates, and image data for leaf area calculation
</commit_message>
<xml_diff>
--- a/test_data/leaf_analysis_results.xlsx
+++ b/test_data/leaf_analysis_results.xlsx
@@ -506,16 +506,16 @@
         <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>124.7658795</v>
+        <v>122.1843434444444</v>
       </c>
       <c r="F2" t="n">
-        <v>141.1986634006824</v>
+        <v>139.1912485363632</v>
       </c>
       <c r="G2" t="n">
-        <v>134.9730839480652</v>
+        <v>132.8801624817497</v>
       </c>
       <c r="H2" t="n">
-        <v>107.8644003001685</v>
+        <v>105.2001676857915</v>
       </c>
     </row>
     <row r="3">
@@ -538,16 +538,16 @@
         <v>2</v>
       </c>
       <c r="E3" t="n">
-        <v>19.86913588888889</v>
+        <v>19.4918965</v>
       </c>
       <c r="F3" t="n">
-        <v>177.6232073011734</v>
+        <v>176.2931171937284</v>
       </c>
       <c r="G3" t="n">
-        <v>169.3917427205563</v>
+        <v>167.9298432102046</v>
       </c>
       <c r="H3" t="n">
-        <v>142.3142981312473</v>
+        <v>140.3173000265745</v>
       </c>
     </row>
     <row r="4">
@@ -570,16 +570,16 @@
         <v>3</v>
       </c>
       <c r="E4" t="n">
-        <v>43.64417794444444</v>
+        <v>42.35923427777777</v>
       </c>
       <c r="F4" t="n">
-        <v>161.3262802204433</v>
+        <v>159.0046392179604</v>
       </c>
       <c r="G4" t="n">
-        <v>149.0200732129209</v>
+        <v>146.3974815673929</v>
       </c>
       <c r="H4" t="n">
-        <v>127.1780441691138</v>
+        <v>123.8850136691243</v>
       </c>
     </row>
     <row r="5">
@@ -602,16 +602,16 @@
         <v>4</v>
       </c>
       <c r="E5" t="n">
-        <v>89.35645211111111</v>
+        <v>87.97294233333332</v>
       </c>
       <c r="F5" t="n">
-        <v>145.1262355767338</v>
+        <v>143.5514876429657</v>
       </c>
       <c r="G5" t="n">
-        <v>138.5760642696806</v>
+        <v>136.9206190514276</v>
       </c>
       <c r="H5" t="n">
-        <v>109.0154176347812</v>
+        <v>106.9026033751899</v>
       </c>
     </row>
     <row r="6">
@@ -634,16 +634,16 @@
         <v>5</v>
       </c>
       <c r="E6" t="n">
-        <v>33.951545</v>
+        <v>33.53846338888889</v>
       </c>
       <c r="F6" t="n">
-        <v>160.8152403524138</v>
+        <v>159.8929558371135</v>
       </c>
       <c r="G6" t="n">
-        <v>150.3187696429491</v>
+        <v>149.2870326920069</v>
       </c>
       <c r="H6" t="n">
-        <v>118.8978824256788</v>
+        <v>117.4816205224464</v>
       </c>
     </row>
     <row r="7">
@@ -666,16 +666,16 @@
         <v>6</v>
       </c>
       <c r="E7" t="n">
-        <v>54.40849333333333</v>
+        <v>50.63520338888888</v>
       </c>
       <c r="F7" t="n">
-        <v>154.5825374290139</v>
+        <v>148.4176239891715</v>
       </c>
       <c r="G7" t="n">
-        <v>145.2542591636551</v>
+        <v>138.810363377642</v>
       </c>
       <c r="H7" t="n">
-        <v>119.2442243159525</v>
+        <v>111.124770069066</v>
       </c>
     </row>
     <row r="8">
@@ -698,16 +698,16 @@
         <v>7</v>
       </c>
       <c r="E8" t="n">
-        <v>196.7603591666667</v>
+        <v>195.2263120555556</v>
       </c>
       <c r="F8" t="n">
-        <v>130.7278969183637</v>
+        <v>129.9096415630648</v>
       </c>
       <c r="G8" t="n">
-        <v>124.586790412687</v>
+        <v>123.737125057893</v>
       </c>
       <c r="H8" t="n">
-        <v>92.97386916561543</v>
+        <v>91.86832187582299</v>
       </c>
     </row>
     <row r="9">
@@ -730,16 +730,16 @@
         <v>1</v>
       </c>
       <c r="E9" t="n">
-        <v>158.2057767777778</v>
+        <v>157.5839142222222</v>
       </c>
       <c r="F9" t="n">
-        <v>163.0631787423667</v>
+        <v>162.7096417880773</v>
       </c>
       <c r="G9" t="n">
-        <v>132.4406007592012</v>
+        <v>131.9747937216264</v>
       </c>
       <c r="H9" t="n">
-        <v>129.1398470594708</v>
+        <v>128.6603227552384</v>
       </c>
     </row>
     <row r="10">
@@ -762,16 +762,16 @@
         <v>2</v>
       </c>
       <c r="E10" t="n">
-        <v>209.9252073888889</v>
+        <v>208.9225212222222</v>
       </c>
       <c r="F10" t="n">
-        <v>162.448000731389</v>
+        <v>161.9610351652206</v>
       </c>
       <c r="G10" t="n">
-        <v>129.7608607119408</v>
+        <v>129.1132702569541</v>
       </c>
       <c r="H10" t="n">
-        <v>122.9407824200667</v>
+        <v>122.2641441682185</v>
       </c>
     </row>
     <row r="11">
@@ -794,16 +794,16 @@
         <v>3</v>
       </c>
       <c r="E11" t="n">
-        <v>243.3373269444444</v>
+        <v>242.4385832222222</v>
       </c>
       <c r="F11" t="n">
-        <v>159.3565403726261</v>
+        <v>158.7293217341082</v>
       </c>
       <c r="G11" t="n">
-        <v>133.1732977629488</v>
+        <v>132.4174565931488</v>
       </c>
       <c r="H11" t="n">
-        <v>120.7507388524956</v>
+        <v>119.9597372125763</v>
       </c>
     </row>
     <row r="12">
@@ -826,16 +826,16 @@
         <v>1</v>
       </c>
       <c r="E12" t="n">
-        <v>206.4476157777778</v>
+        <v>205.6071156666667</v>
       </c>
       <c r="F12" t="n">
-        <v>133.0581530647778</v>
+        <v>132.6320883431398</v>
       </c>
       <c r="G12" t="n">
-        <v>122.1397898777826</v>
+        <v>121.6767289161763</v>
       </c>
       <c r="H12" t="n">
-        <v>106.0644635258746</v>
+        <v>105.5321480344504</v>
       </c>
     </row>
     <row r="13">
@@ -858,16 +858,16 @@
         <v>2</v>
       </c>
       <c r="E13" t="n">
-        <v>103.515922</v>
+        <v>102.6897587777778</v>
       </c>
       <c r="F13" t="n">
-        <v>141.9823867176318</v>
+        <v>141.1995044211741</v>
       </c>
       <c r="G13" t="n">
-        <v>135.1748194049203</v>
+        <v>134.3499092004548</v>
       </c>
       <c r="H13" t="n">
-        <v>123.6080455318504</v>
+        <v>122.6828804670661</v>
       </c>
     </row>
     <row r="14">
@@ -890,16 +890,16 @@
         <v>3</v>
       </c>
       <c r="E14" t="n">
-        <v>188.5981891111111</v>
+        <v>187.5632449444444</v>
       </c>
       <c r="F14" t="n">
-        <v>127.5922500162192</v>
+        <v>127.0267623351815</v>
       </c>
       <c r="G14" t="n">
-        <v>122.7419483396202</v>
+        <v>122.1603690071285</v>
       </c>
       <c r="H14" t="n">
-        <v>109.966903621046</v>
+        <v>109.3103200857289</v>
       </c>
     </row>
     <row r="15">
@@ -922,16 +922,16 @@
         <v>4</v>
       </c>
       <c r="E15" t="n">
-        <v>214.1142671111111</v>
+        <v>213.3248421666667</v>
       </c>
       <c r="F15" t="n">
-        <v>117.2368507264656</v>
+        <v>116.8066467740212</v>
       </c>
       <c r="G15" t="n">
-        <v>115.7841569886485</v>
+        <v>115.3572209481065</v>
       </c>
       <c r="H15" t="n">
-        <v>104.3560009172959</v>
+        <v>103.8840719094474</v>
       </c>
     </row>
     <row r="16">
@@ -954,16 +954,16 @@
         <v>5</v>
       </c>
       <c r="E16" t="n">
-        <v>226.1939920555556</v>
+        <v>225.1196214444444</v>
       </c>
       <c r="F16" t="n">
-        <v>122.6848031771989</v>
+        <v>122.1103998747946</v>
       </c>
       <c r="G16" t="n">
-        <v>121.7302807304443</v>
+        <v>121.1579388058533</v>
       </c>
       <c r="H16" t="n">
-        <v>96.90362496593077</v>
+        <v>96.21099460051647</v>
       </c>
     </row>
     <row r="17">
@@ -986,16 +986,16 @@
         <v>6</v>
       </c>
       <c r="E17" t="n">
-        <v>58.11726727777778</v>
+        <v>57.87802044444444</v>
       </c>
       <c r="F17" t="n">
-        <v>153.4929122555177</v>
+        <v>153.1185214101255</v>
       </c>
       <c r="G17" t="n">
-        <v>147.5887911956457</v>
+        <v>147.1944928232539</v>
       </c>
       <c r="H17" t="n">
-        <v>133.4936599078892</v>
+        <v>133.0371449162213</v>
       </c>
     </row>
     <row r="18">
@@ -1018,16 +1018,16 @@
         <v>7</v>
       </c>
       <c r="E18" t="n">
-        <v>120.8312995555555</v>
+        <v>120.1807632222222</v>
       </c>
       <c r="F18" t="n">
-        <v>131.6633647639813</v>
+        <v>131.0830792904219</v>
       </c>
       <c r="G18" t="n">
-        <v>127.604508107952</v>
+        <v>127.0119327584705</v>
       </c>
       <c r="H18" t="n">
-        <v>113.506404054698</v>
+        <v>112.8336962517783</v>
       </c>
     </row>
     <row r="19">
@@ -1050,16 +1050,16 @@
         <v>8</v>
       </c>
       <c r="E19" t="n">
-        <v>152.2183335555555</v>
+        <v>151.4154677777778</v>
       </c>
       <c r="F19" t="n">
-        <v>121.2302768424561</v>
+        <v>120.6487460579667</v>
       </c>
       <c r="G19" t="n">
-        <v>119.4849282324143</v>
+        <v>118.9034505065441</v>
       </c>
       <c r="H19" t="n">
-        <v>106.1511658641415</v>
+        <v>105.4951424907875</v>
       </c>
     </row>
     <row r="20">
@@ -1082,16 +1082,16 @@
         <v>1</v>
       </c>
       <c r="E20" t="n">
-        <v>112.515904</v>
+        <v>112.5732515555555</v>
       </c>
       <c r="F20" t="n">
-        <v>133.1634618381276</v>
+        <v>132.9046283746943</v>
       </c>
       <c r="G20" t="n">
-        <v>134.0253996945804</v>
+        <v>133.746023585861</v>
       </c>
       <c r="H20" t="n">
-        <v>111.7962258858728</v>
+        <v>111.5390319515197</v>
       </c>
     </row>
     <row r="21">
@@ -1114,16 +1114,16 @@
         <v>2</v>
       </c>
       <c r="E21" t="n">
-        <v>189.4431695</v>
+        <v>188.2057167777778</v>
       </c>
       <c r="F21" t="n">
-        <v>117.8539203658265</v>
+        <v>117.0856105752589</v>
       </c>
       <c r="G21" t="n">
-        <v>118.2745836121645</v>
+        <v>117.5198473211028</v>
       </c>
       <c r="H21" t="n">
-        <v>106.3404714105138</v>
+        <v>105.5052904360517</v>
       </c>
     </row>
     <row r="22">
@@ -1146,16 +1146,16 @@
         <v>3</v>
       </c>
       <c r="E22" t="n">
-        <v>94.00518833333332</v>
+        <v>93.30805711111111</v>
       </c>
       <c r="F22" t="n">
-        <v>141.1565925870684</v>
+        <v>140.4422011456475</v>
       </c>
       <c r="G22" t="n">
-        <v>134.2538407040048</v>
+        <v>133.4983003098882</v>
       </c>
       <c r="H22" t="n">
-        <v>119.2198150495935</v>
+        <v>118.3403512066861</v>
       </c>
     </row>
     <row r="23">
@@ -1178,16 +1178,16 @@
         <v>4</v>
       </c>
       <c r="E23" t="n">
-        <v>109.4307847222222</v>
+        <v>108.4899263888889</v>
       </c>
       <c r="F23" t="n">
-        <v>118.139602784997</v>
+        <v>117.2113225253212</v>
       </c>
       <c r="G23" t="n">
-        <v>116.0958385471813</v>
+        <v>115.1643206161214</v>
       </c>
       <c r="H23" t="n">
-        <v>103.9472519010492</v>
+        <v>102.8951558101155</v>
       </c>
     </row>
     <row r="24">
@@ -1210,16 +1210,16 @@
         <v>5</v>
       </c>
       <c r="E24" t="n">
-        <v>215.5255546111111</v>
+        <v>212.0058483888889</v>
       </c>
       <c r="F24" t="n">
-        <v>128.4722771629861</v>
+        <v>126.8439642064857</v>
       </c>
       <c r="G24" t="n">
-        <v>129.5116056687971</v>
+        <v>127.9285209834077</v>
       </c>
       <c r="H24" t="n">
-        <v>112.5205959756117</v>
+        <v>110.6665503460538</v>
       </c>
     </row>
     <row r="25">
@@ -1242,16 +1242,16 @@
         <v>6</v>
       </c>
       <c r="E25" t="n">
-        <v>161.8034398333333</v>
+        <v>160.3589982777778</v>
       </c>
       <c r="F25" t="n">
-        <v>131.020102359039</v>
+        <v>130.1417937445871</v>
       </c>
       <c r="G25" t="n">
-        <v>132.6534679285877</v>
+        <v>131.8105068134229</v>
       </c>
       <c r="H25" t="n">
-        <v>110.0889176237925</v>
+        <v>109.0558887049563</v>
       </c>
     </row>
     <row r="26">
@@ -1274,16 +1274,16 @@
         <v>7</v>
       </c>
       <c r="E26" t="n">
-        <v>187.5524922777778</v>
+        <v>187.2621702777778</v>
       </c>
       <c r="F26" t="n">
-        <v>120.7146904087414</v>
+        <v>120.4181161674727</v>
       </c>
       <c r="G26" t="n">
-        <v>118.1009759724431</v>
+        <v>117.8011237755843</v>
       </c>
       <c r="H26" t="n">
-        <v>102.3845256133944</v>
+        <v>102.057225820441</v>
       </c>
     </row>
     <row r="27">
@@ -1306,16 +1306,16 @@
         <v>8</v>
       </c>
       <c r="E27" t="n">
-        <v>213.38667</v>
+        <v>212.8373879444444</v>
       </c>
       <c r="F27" t="n">
-        <v>117.9541571212359</v>
+        <v>117.5763199575424</v>
       </c>
       <c r="G27" t="n">
-        <v>117.7711908562355</v>
+        <v>117.392674411855</v>
       </c>
       <c r="H27" t="n">
-        <v>102.0609529165598</v>
+        <v>101.6468061463957</v>
       </c>
     </row>
     <row r="28">
@@ -1338,16 +1338,16 @@
         <v>1</v>
       </c>
       <c r="E28" t="n">
-        <v>59.87532827777778</v>
+        <v>59.63339327777778</v>
       </c>
       <c r="F28" t="n">
-        <v>104.3960700757576</v>
+        <v>103.8275985024068</v>
       </c>
       <c r="G28" t="n">
-        <v>101.4372040719697</v>
+        <v>100.8633743388602</v>
       </c>
       <c r="H28" t="n">
-        <v>90.46801017992425</v>
+        <v>89.84272300469483</v>
       </c>
     </row>
     <row r="29">
@@ -1370,16 +1370,16 @@
         <v>2</v>
       </c>
       <c r="E29" t="n">
-        <v>180.8777744444444</v>
+        <v>179.8741922222222</v>
       </c>
       <c r="F29" t="n">
-        <v>86.11823440297479</v>
+        <v>85.34874955482569</v>
       </c>
       <c r="G29" t="n">
-        <v>87.12927184370511</v>
+        <v>86.39444422460528</v>
       </c>
       <c r="H29" t="n">
-        <v>74.08734530859583</v>
+        <v>73.25748882117843</v>
       </c>
     </row>
     <row r="30">
@@ -1402,16 +1402,16 @@
         <v>3</v>
       </c>
       <c r="E30" t="n">
-        <v>91.21755949999999</v>
+        <v>90.32956844444443</v>
       </c>
       <c r="F30" t="n">
-        <v>93.78282523686309</v>
+        <v>92.46815449294722</v>
       </c>
       <c r="G30" t="n">
-        <v>94.61364564891734</v>
+        <v>93.34552669836155</v>
       </c>
       <c r="H30" t="n">
-        <v>80.43082819400401</v>
+        <v>79.01347687713645</v>
       </c>
     </row>
     <row r="31">
@@ -1434,16 +1434,16 @@
         <v>4</v>
       </c>
       <c r="E31" t="n">
-        <v>243.4968248333333</v>
+        <v>241.4179759444444</v>
       </c>
       <c r="F31" t="n">
-        <v>82.79602448496018</v>
+        <v>81.60369340189908</v>
       </c>
       <c r="G31" t="n">
-        <v>84.2335944184822</v>
+        <v>83.10999786039443</v>
       </c>
       <c r="H31" t="n">
-        <v>71.25727491461711</v>
+        <v>69.99183260906455</v>
       </c>
     </row>
     <row r="32">
@@ -1466,16 +1466,16 @@
         <v>5</v>
       </c>
       <c r="E32" t="n">
-        <v>83.25969011111111</v>
+        <v>82.75879505555555</v>
       </c>
       <c r="F32" t="n">
-        <v>124.7410777065178</v>
+        <v>124.0812218649518</v>
       </c>
       <c r="G32" t="n">
-        <v>120.523554854793</v>
+        <v>119.8485316184351</v>
       </c>
       <c r="H32" t="n">
-        <v>106.1716915603094</v>
+        <v>105.3982851018221</v>
       </c>
     </row>
     <row r="33">
@@ -1498,16 +1498,16 @@
         <v>6</v>
       </c>
       <c r="E33" t="n">
-        <v>96.75339072222222</v>
+        <v>96.76414338888888</v>
       </c>
       <c r="F33" t="n">
-        <v>95.37192782805015</v>
+        <v>95.37519729838857</v>
       </c>
       <c r="G33" t="n">
-        <v>97.67959472109543</v>
+        <v>97.68624967881658</v>
       </c>
       <c r="H33" t="n">
-        <v>80.46526311925258</v>
+        <v>80.4728003523841</v>
       </c>
     </row>
     <row r="34">
@@ -1530,16 +1530,16 @@
         <v>7</v>
       </c>
       <c r="E34" t="n">
-        <v>83.27313094444445</v>
+        <v>82.84302427777777</v>
       </c>
       <c r="F34" t="n">
-        <v>104.0749850924269</v>
+        <v>103.3837903795517</v>
       </c>
       <c r="G34" t="n">
-        <v>104.1531433682596</v>
+        <v>103.4741292573802</v>
       </c>
       <c r="H34" t="n">
-        <v>92.08737967458897</v>
+        <v>91.34007663819494</v>
       </c>
     </row>
     <row r="35">
@@ -1562,16 +1562,16 @@
         <v>8</v>
       </c>
       <c r="E35" t="n">
-        <v>74.17189466666666</v>
+        <v>74.0661601111111</v>
       </c>
       <c r="F35" t="n">
-        <v>99.47904406487727</v>
+        <v>99.27248987805754</v>
       </c>
       <c r="G35" t="n">
-        <v>100.2077412563992</v>
+        <v>100.0067080328694</v>
       </c>
       <c r="H35" t="n">
-        <v>85.79048849337352</v>
+        <v>85.56551112814739</v>
       </c>
     </row>
     <row r="36">
@@ -1594,16 +1594,16 @@
         <v>9</v>
       </c>
       <c r="E36" t="n">
-        <v>201.0730745555555</v>
+        <v>200.1976282777778</v>
       </c>
       <c r="F36" t="n">
-        <v>86.32694879083319</v>
+        <v>85.68339366556083</v>
       </c>
       <c r="G36" t="n">
-        <v>87.28579018675451</v>
+        <v>86.66863821120134</v>
       </c>
       <c r="H36" t="n">
-        <v>72.19816876090287</v>
+        <v>71.50160540054966</v>
       </c>
     </row>
     <row r="37">
@@ -1626,16 +1626,16 @@
         <v>10</v>
       </c>
       <c r="E37" t="n">
-        <v>99.37972955555556</v>
+        <v>97.58045</v>
       </c>
       <c r="F37" t="n">
-        <v>105.7390139813938</v>
+        <v>103.2926092965738</v>
       </c>
       <c r="G37" t="n">
-        <v>107.4035855222042</v>
+        <v>105.0311704371863</v>
       </c>
       <c r="H37" t="n">
-        <v>89.24980804599753</v>
+        <v>86.54679202735142</v>
       </c>
     </row>
     <row r="38">
@@ -1658,16 +1658,16 @@
         <v>1</v>
       </c>
       <c r="E38" t="n">
-        <v>35.41390766666667</v>
+        <v>33.75889305555555</v>
       </c>
       <c r="F38" t="n">
-        <v>189.6640011631288</v>
+        <v>186.8347199675325</v>
       </c>
       <c r="G38" t="n">
-        <v>183.8685179800329</v>
+        <v>180.8682021103896</v>
       </c>
       <c r="H38" t="n">
-        <v>165.3272753707473</v>
+        <v>161.5346996753247</v>
       </c>
     </row>
     <row r="39">
@@ -1690,16 +1690,16 @@
         <v>2</v>
       </c>
       <c r="E39" t="n">
-        <v>51.14595505555555</v>
+        <v>49.42552838888889</v>
       </c>
       <c r="F39" t="n">
-        <v>164.1487617362907</v>
+        <v>161.2436605352935</v>
       </c>
       <c r="G39" t="n">
-        <v>152.9219621717241</v>
+        <v>149.7028804558084</v>
       </c>
       <c r="H39" t="n">
-        <v>136.0287794257722</v>
+        <v>132.2152076812155</v>
       </c>
     </row>
     <row r="40">
@@ -1722,16 +1722,16 @@
         <v>3</v>
       </c>
       <c r="E40" t="n">
-        <v>31.42646044444444</v>
+        <v>30.80280577777778</v>
       </c>
       <c r="F40" t="n">
-        <v>176.6445497630332</v>
+        <v>175.2988479910087</v>
       </c>
       <c r="G40" t="n">
-        <v>162.9472059958117</v>
+        <v>161.3611688676594</v>
       </c>
       <c r="H40" t="n">
-        <v>143.3639920643668</v>
+        <v>141.3636976678842</v>
       </c>
     </row>
     <row r="41">
@@ -1754,16 +1754,16 @@
         <v>4</v>
       </c>
       <c r="E41" t="n">
-        <v>42.4273345</v>
+        <v>41.14418294444445</v>
       </c>
       <c r="F41" t="n">
-        <v>181.4963607530598</v>
+        <v>179.4542408376963</v>
       </c>
       <c r="G41" t="n">
-        <v>173.3135038425568</v>
+        <v>171.0860732984293</v>
       </c>
       <c r="H41" t="n">
-        <v>158.2843492050584</v>
+        <v>155.642387434555</v>
       </c>
     </row>
     <row r="42">
@@ -1786,16 +1786,16 @@
         <v>5</v>
       </c>
       <c r="E42" t="n">
-        <v>34.60387344444445</v>
+        <v>32.8144505</v>
       </c>
       <c r="F42" t="n">
-        <v>184.7866513692822</v>
+        <v>181.4484208313627</v>
       </c>
       <c r="G42" t="n">
-        <v>168.862772484661</v>
+        <v>164.79321036313</v>
       </c>
       <c r="H42" t="n">
-        <v>162.2491644635107</v>
+        <v>157.7799674181512</v>
       </c>
     </row>
     <row r="43">
@@ -1818,16 +1818,16 @@
         <v>6</v>
       </c>
       <c r="E43" t="n">
-        <v>163.6959091666667</v>
+        <v>162.0606077777778</v>
       </c>
       <c r="F43" t="n">
-        <v>139.6839701579555</v>
+        <v>138.657103601688</v>
       </c>
       <c r="G43" t="n">
-        <v>139.5621835220954</v>
+        <v>138.5482133315886</v>
       </c>
       <c r="H43" t="n">
-        <v>120.6744258861381</v>
+        <v>119.4775862256971</v>
       </c>
     </row>
     <row r="44">
@@ -1850,16 +1850,16 @@
         <v>7</v>
       </c>
       <c r="E44" t="n">
-        <v>422.4884023333333</v>
+        <v>419.6335693333333</v>
       </c>
       <c r="F44" t="n">
-        <v>98.91456916909682</v>
+        <v>97.93694501673146</v>
       </c>
       <c r="G44" t="n">
-        <v>94.67928246674118</v>
+        <v>93.70520050257846</v>
       </c>
       <c r="H44" t="n">
-        <v>82.79403484297131</v>
+        <v>81.7428727351183</v>
       </c>
     </row>
     <row r="45">
@@ -1882,16 +1882,16 @@
         <v>8</v>
       </c>
       <c r="E45" t="n">
-        <v>78.20593677777778</v>
+        <v>76.65396855555555</v>
       </c>
       <c r="F45" t="n">
-        <v>130.5918573577957</v>
+        <v>128.2773095772455</v>
       </c>
       <c r="G45" t="n">
-        <v>125.8934225595652</v>
+        <v>123.6014519305638</v>
       </c>
       <c r="H45" t="n">
-        <v>108.0103074262873</v>
+        <v>105.4278843951816</v>
       </c>
     </row>
     <row r="46">
@@ -1914,16 +1914,16 @@
         <v>1</v>
       </c>
       <c r="E46" t="n">
-        <v>77.57063338888888</v>
+        <v>75.83049349999999</v>
       </c>
       <c r="F46" t="n">
-        <v>185.6594486866561</v>
+        <v>184.3669619760547</v>
       </c>
       <c r="G46" t="n">
-        <v>169.4625926506483</v>
+        <v>167.8747567703683</v>
       </c>
       <c r="H46" t="n">
-        <v>136.0848691134649</v>
+        <v>133.7717189753451</v>
       </c>
     </row>
     <row r="47">
@@ -1946,16 +1946,16 @@
         <v>2</v>
       </c>
       <c r="E47" t="n">
-        <v>62.53392511111111</v>
+        <v>61.06260188888889</v>
       </c>
       <c r="F47" t="n">
-        <v>186.3429565986131</v>
+        <v>184.995137396811</v>
       </c>
       <c r="G47" t="n">
-        <v>175.1679973478465</v>
+        <v>173.6202646160805</v>
       </c>
       <c r="H47" t="n">
-        <v>145.3643948393513</v>
+        <v>143.137396811037</v>
       </c>
     </row>
     <row r="48">
@@ -1978,16 +1978,16 @@
         <v>3</v>
       </c>
       <c r="E48" t="n">
-        <v>83.66649933333333</v>
+        <v>82.70413566666666</v>
       </c>
       <c r="F48" t="n">
-        <v>179.7154314446591</v>
+        <v>178.9399873923093</v>
       </c>
       <c r="G48" t="n">
-        <v>160.8451868935569</v>
+        <v>159.8838201302795</v>
       </c>
       <c r="H48" t="n">
-        <v>130.2424317978765</v>
+        <v>128.9358898928346</v>
       </c>
     </row>
     <row r="49">
@@ -2010,16 +2010,16 @@
         <v>1</v>
       </c>
       <c r="E49" t="n">
-        <v>208.8508367777778</v>
+        <v>207.4279005555555</v>
       </c>
       <c r="F49" t="n">
-        <v>137.2551572100353</v>
+        <v>136.6003780526911</v>
       </c>
       <c r="G49" t="n">
-        <v>132.9559593961391</v>
+        <v>132.2831766552463</v>
       </c>
       <c r="H49" t="n">
-        <v>107.0040486508688</v>
+        <v>106.1567315319573</v>
       </c>
     </row>
     <row r="50">
@@ -2042,16 +2042,16 @@
         <v>2</v>
       </c>
       <c r="E50" t="n">
-        <v>297.3578282222222</v>
+        <v>295.9877592777777</v>
       </c>
       <c r="F50" t="n">
-        <v>131.8090236319143</v>
+        <v>131.3236682560701</v>
       </c>
       <c r="G50" t="n">
-        <v>127.1620423459315</v>
+        <v>126.6613026774422</v>
       </c>
       <c r="H50" t="n">
-        <v>100.063371123905</v>
+        <v>99.44126431799152</v>
       </c>
     </row>
     <row r="51">
@@ -2074,16 +2074,16 @@
         <v>3</v>
       </c>
       <c r="E51" t="n">
-        <v>63.16564427777777</v>
+        <v>62.43446294444444</v>
       </c>
       <c r="F51" t="n">
-        <v>157.1362574545854</v>
+        <v>156.1588003113187</v>
       </c>
       <c r="G51" t="n">
-        <v>155.7855277983895</v>
+        <v>154.8027851901267</v>
       </c>
       <c r="H51" t="n">
-        <v>129.3887377360046</v>
+        <v>128.1092116966867</v>
       </c>
     </row>
     <row r="52">
@@ -2106,16 +2106,16 @@
         <v>4</v>
       </c>
       <c r="E52" t="n">
-        <v>79.26865866666667</v>
+        <v>78.57331955555556</v>
       </c>
       <c r="F52" t="n">
-        <v>146.9557692728986</v>
+        <v>146.1895660243946</v>
       </c>
       <c r="G52" t="n">
-        <v>143.1335903783381</v>
+        <v>142.3450371221496</v>
       </c>
       <c r="H52" t="n">
-        <v>126.402238920411</v>
+        <v>125.4643362206116</v>
       </c>
     </row>
     <row r="53">
@@ -2138,16 +2138,16 @@
         <v>5</v>
       </c>
       <c r="E53" t="n">
-        <v>59.17282072222222</v>
+        <v>58.435367</v>
       </c>
       <c r="F53" t="n">
-        <v>145.59911176906</v>
+        <v>144.4337360232621</v>
       </c>
       <c r="G53" t="n">
-        <v>146.2549814951888</v>
+        <v>145.1165202793849</v>
       </c>
       <c r="H53" t="n">
-        <v>122.2369207994079</v>
+        <v>120.8007434275608</v>
       </c>
     </row>
     <row r="54">
@@ -2170,16 +2170,16 @@
         <v>6</v>
       </c>
       <c r="E54" t="n">
-        <v>107.9540851666667</v>
+        <v>106.6655572777778</v>
       </c>
       <c r="F54" t="n">
-        <v>136.1303547793524</v>
+        <v>135.0916024301019</v>
       </c>
       <c r="G54" t="n">
-        <v>131.7611615069245</v>
+        <v>130.7004507447086</v>
       </c>
       <c r="H54" t="n">
-        <v>115.9870549117087</v>
+        <v>114.7352201463287</v>
       </c>
     </row>
     <row r="55">
@@ -2202,16 +2202,16 @@
         <v>7</v>
       </c>
       <c r="E55" t="n">
-        <v>70.95505522222221</v>
+        <v>70.30272677777778</v>
       </c>
       <c r="F55" t="n">
-        <v>153.8820283955764</v>
+        <v>153.0543376057802</v>
       </c>
       <c r="G55" t="n">
-        <v>154.0806503028371</v>
+        <v>153.264017419706</v>
       </c>
       <c r="H55" t="n">
-        <v>125.6301218704789</v>
+        <v>124.5676250804177</v>
       </c>
     </row>
     <row r="56">
@@ -2234,16 +2234,16 @@
         <v>8</v>
       </c>
       <c r="E56" t="n">
-        <v>115.7470803333333</v>
+        <v>114.451384</v>
       </c>
       <c r="F56" t="n">
-        <v>138.9226940590914</v>
+        <v>137.8574946843498</v>
       </c>
       <c r="G56" t="n">
-        <v>139.4420356726827</v>
+        <v>138.399094427363</v>
       </c>
       <c r="H56" t="n">
-        <v>109.3214020967913</v>
+        <v>107.9484955562694</v>
       </c>
     </row>
     <row r="57">
@@ -2266,16 +2266,16 @@
         <v>9</v>
       </c>
       <c r="E57" t="n">
-        <v>117.4648188333333</v>
+        <v>116.5257526111111</v>
       </c>
       <c r="F57" t="n">
-        <v>146.5051771846827</v>
+        <v>145.7609608348828</v>
       </c>
       <c r="G57" t="n">
-        <v>146.1955428605433</v>
+        <v>145.4578060337072</v>
       </c>
       <c r="H57" t="n">
-        <v>115.4830848879764</v>
+        <v>114.505532897499</v>
       </c>
     </row>
     <row r="58">
@@ -2298,16 +2298,16 @@
         <v>1</v>
       </c>
       <c r="E58" t="n">
-        <v>80.78120044444444</v>
+        <v>80.26417638888888</v>
       </c>
       <c r="F58" t="n">
-        <v>133.364273281114</v>
+        <v>132.6987801406014</v>
       </c>
       <c r="G58" t="n">
-        <v>132.7422541340296</v>
+        <v>132.081710869232</v>
       </c>
       <c r="H58" t="n">
-        <v>101.0516318537859</v>
+        <v>100.1818181818182</v>
       </c>
     </row>
     <row r="59">
@@ -2330,16 +2330,16 @@
         <v>2</v>
       </c>
       <c r="E59" t="n">
-        <v>95.34031111111111</v>
+        <v>96.51772811111111</v>
       </c>
       <c r="F59" t="n">
-        <v>127.6325046601332</v>
+        <v>128.3664745787439</v>
       </c>
       <c r="G59" t="n">
-        <v>127.4716977649816</v>
+        <v>128.1340360347217</v>
       </c>
       <c r="H59" t="n">
-        <v>95.4205008951147</v>
+        <v>96.45936975709388</v>
       </c>
     </row>
     <row r="60">
@@ -2362,16 +2362,16 @@
         <v>3</v>
       </c>
       <c r="E60" t="n">
-        <v>165.2380207777778</v>
+        <v>165.4656188888889</v>
       </c>
       <c r="F60" t="n">
-        <v>124.5235815357055</v>
+        <v>124.3344733169261</v>
       </c>
       <c r="G60" t="n">
-        <v>124.7409816487348</v>
+        <v>124.5305718029853</v>
       </c>
       <c r="H60" t="n">
-        <v>97.03117902346958</v>
+        <v>96.83835671897806</v>
       </c>
     </row>
     <row r="61">
@@ -2394,16 +2394,16 @@
         <v>1</v>
       </c>
       <c r="E61" t="n">
-        <v>385.7940312777778</v>
+        <v>384.2393748888888</v>
       </c>
       <c r="F61" t="n">
-        <v>112.1250178025866</v>
+        <v>111.6575980663493</v>
       </c>
       <c r="G61" t="n">
-        <v>111.9434911446489</v>
+        <v>111.4865862208938</v>
       </c>
       <c r="H61" t="n">
-        <v>107.4023935864746</v>
+        <v>106.9215976604303</v>
       </c>
     </row>
     <row r="62">
@@ -2426,16 +2426,16 @@
         <v>2</v>
       </c>
       <c r="E62" t="n">
-        <v>272.5075195</v>
+        <v>271.7073418888889</v>
       </c>
       <c r="F62" t="n">
-        <v>114.1481961518771</v>
+        <v>113.7890693548073</v>
       </c>
       <c r="G62" t="n">
-        <v>114.2743585921754</v>
+        <v>113.9195052677417</v>
       </c>
       <c r="H62" t="n">
-        <v>108.1411259226617</v>
+        <v>107.7619734695602</v>
       </c>
     </row>
     <row r="63">
@@ -2458,16 +2458,16 @@
         <v>3</v>
       </c>
       <c r="E63" t="n">
-        <v>49.19882633333333</v>
+        <v>48.79649738888889</v>
       </c>
       <c r="F63" t="n">
-        <v>146.4419222324527</v>
+        <v>145.670772196637</v>
       </c>
       <c r="G63" t="n">
-        <v>136.8959558042354</v>
+        <v>136.0555139052515</v>
       </c>
       <c r="H63" t="n">
-        <v>132.4093774346625</v>
+        <v>131.516047267145</v>
       </c>
     </row>
     <row r="64">
@@ -2490,16 +2490,16 @@
         <v>4</v>
       </c>
       <c r="E64" t="n">
-        <v>56.84755655555555</v>
+        <v>56.65132038888888</v>
       </c>
       <c r="F64" t="n">
-        <v>121.5693985357264</v>
+        <v>121.1527278363298</v>
       </c>
       <c r="G64" t="n">
-        <v>108.0544005436965</v>
+        <v>107.5948543087415</v>
       </c>
       <c r="H64" t="n">
-        <v>104.7016465354793</v>
+        <v>104.2213267203968</v>
       </c>
     </row>
     <row r="65">
@@ -2522,16 +2522,16 @@
         <v>5</v>
       </c>
       <c r="E65" t="n">
-        <v>125.7237628888889</v>
+        <v>125.2327244444444</v>
       </c>
       <c r="F65" t="n">
-        <v>114.5083375584474</v>
+        <v>114.0006504616864</v>
       </c>
       <c r="G65" t="n">
-        <v>110.0990225902766</v>
+        <v>109.5773413085592</v>
       </c>
       <c r="H65" t="n">
-        <v>100.3296856515126</v>
+        <v>99.75942815933483</v>
       </c>
     </row>
     <row r="66">
@@ -2554,16 +2554,16 @@
         <v>6</v>
       </c>
       <c r="E66" t="n">
-        <v>142.5785678888889</v>
+        <v>141.1153091666667</v>
       </c>
       <c r="F66" t="n">
-        <v>134.7942614813271</v>
+        <v>133.8311130370187</v>
       </c>
       <c r="G66" t="n">
-        <v>132.9343293826374</v>
+        <v>131.9716726507367</v>
       </c>
       <c r="H66" t="n">
-        <v>126.4555025800047</v>
+        <v>125.4248607156122</v>
       </c>
     </row>
     <row r="67">
@@ -2586,16 +2586,16 @@
         <v>7</v>
       </c>
       <c r="E67" t="n">
-        <v>223.3337827222222</v>
+        <v>222.0927457777778</v>
       </c>
       <c r="F67" t="n">
-        <v>113.1087880935507</v>
+        <v>112.4544482717662</v>
       </c>
       <c r="G67" t="n">
-        <v>112.6740058272305</v>
+        <v>112.0297660054638</v>
       </c>
       <c r="H67" t="n">
-        <v>107.1230254350736</v>
+        <v>106.4387061012789</v>
       </c>
     </row>
     <row r="68">
@@ -2618,16 +2618,16 @@
         <v>8</v>
       </c>
       <c r="E68" t="n">
-        <v>289.9098144444444</v>
+        <v>288.192972</v>
       </c>
       <c r="F68" t="n">
-        <v>122.6062581565083</v>
+        <v>121.983482224248</v>
       </c>
       <c r="G68" t="n">
-        <v>115.6449381313742</v>
+        <v>114.9980249164388</v>
       </c>
       <c r="H68" t="n">
-        <v>116.5425407221229</v>
+        <v>115.8936068064418</v>
       </c>
     </row>
     <row r="69">
@@ -2650,16 +2650,16 @@
         <v>9</v>
       </c>
       <c r="E69" t="n">
-        <v>67.47298333333333</v>
+        <v>66.85828922222221</v>
       </c>
       <c r="F69" t="n">
-        <v>127.1493572001345</v>
+        <v>126.2512724140631</v>
       </c>
       <c r="G69" t="n">
-        <v>116.511497969425</v>
+        <v>115.5360060553859</v>
       </c>
       <c r="H69" t="n">
-        <v>117.8854859153108</v>
+        <v>116.89979902383</v>
       </c>
     </row>
     <row r="70">
@@ -2682,16 +2682,16 @@
         <v>1</v>
       </c>
       <c r="E70" t="n">
-        <v>17.81896077777778</v>
+        <v>16.85838922222222</v>
       </c>
       <c r="F70" t="n">
-        <v>192.1113691340107</v>
+        <v>189.4342145554762</v>
       </c>
       <c r="G70" t="n">
-        <v>188.3802612481858</v>
+        <v>185.5586404001225</v>
       </c>
       <c r="H70" t="n">
-        <v>168.7328495403967</v>
+        <v>164.7793202000612</v>
       </c>
     </row>
     <row r="71">
@@ -2714,16 +2714,16 @@
         <v>2</v>
       </c>
       <c r="E71" t="n">
-        <v>62.42371027777777</v>
+        <v>61.34665149999999</v>
       </c>
       <c r="F71" t="n">
-        <v>150.6132363759833</v>
+        <v>149.0994673959983</v>
       </c>
       <c r="G71" t="n">
-        <v>144.4394488144417</v>
+        <v>142.8616956959839</v>
       </c>
       <c r="H71" t="n">
-        <v>133.0473657404787</v>
+        <v>131.246293364042</v>
       </c>
     </row>
     <row r="72">
@@ -2746,16 +2746,16 @@
         <v>3</v>
       </c>
       <c r="E72" t="n">
-        <v>14.63079511111111</v>
+        <v>14.25982811111111</v>
       </c>
       <c r="F72" t="n">
-        <v>165.1060195547179</v>
+        <v>163.0293868666102</v>
       </c>
       <c r="G72" t="n">
-        <v>161.8977500294499</v>
+        <v>159.7667190712299</v>
       </c>
       <c r="H72" t="n">
-        <v>144.6351749322653</v>
+        <v>141.9955254565244</v>
       </c>
     </row>
     <row r="73">
@@ -2778,16 +2778,16 @@
         <v>4</v>
       </c>
       <c r="E73" t="n">
-        <v>26.58596833333333</v>
+        <v>25.177369</v>
       </c>
       <c r="F73" t="n">
-        <v>180.0401645768025</v>
+        <v>176.7543376480309</v>
       </c>
       <c r="G73" t="n">
-        <v>174.3505094043887</v>
+        <v>170.8477003580281</v>
       </c>
       <c r="H73" t="n">
-        <v>159.5476097178683</v>
+        <v>155.2015973561003</v>
       </c>
     </row>
     <row r="74">
@@ -2810,16 +2810,16 @@
         <v>5</v>
       </c>
       <c r="E74" t="n">
-        <v>259.9493008888889</v>
+        <v>257.2459012777778</v>
       </c>
       <c r="F74" t="n">
-        <v>92.61742087937606</v>
+        <v>91.25723947550034</v>
       </c>
       <c r="G74" t="n">
-        <v>95.1827116143749</v>
+        <v>93.86371980676329</v>
       </c>
       <c r="H74" t="n">
-        <v>80.42733332422723</v>
+        <v>78.9431884057971</v>
       </c>
     </row>
     <row r="75">
@@ -2842,16 +2842,16 @@
         <v>6</v>
       </c>
       <c r="E75" t="n">
-        <v>139.2981085</v>
+        <v>138.0660321111111</v>
       </c>
       <c r="F75" t="n">
-        <v>98.59493429580866</v>
+        <v>97.45645233668824</v>
       </c>
       <c r="G75" t="n">
-        <v>100.4684823221412</v>
+        <v>99.36263863068145</v>
       </c>
       <c r="H75" t="n">
-        <v>82.13647917037338</v>
+        <v>80.86179883325855</v>
       </c>
     </row>
     <row r="76">
@@ -2874,16 +2874,16 @@
         <v>7</v>
       </c>
       <c r="E76" t="n">
-        <v>87.1790371111111</v>
+        <v>85.68172827777778</v>
       </c>
       <c r="F76" t="n">
-        <v>146.1878267212384</v>
+        <v>144.5381903642773</v>
       </c>
       <c r="G76" t="n">
-        <v>141.6056854560927</v>
+        <v>139.9348753788113</v>
       </c>
       <c r="H76" t="n">
-        <v>132.4978725128663</v>
+        <v>130.6508132846806</v>
       </c>
     </row>
     <row r="77">
@@ -2906,16 +2906,16 @@
         <v>8</v>
       </c>
       <c r="E77" t="n">
-        <v>21.60569155555556</v>
+        <v>21.47397138888889</v>
       </c>
       <c r="F77" t="n">
-        <v>149.8623101036894</v>
+        <v>149.3161895519974</v>
       </c>
       <c r="G77" t="n">
-        <v>146.4448195482678</v>
+        <v>145.8821769367621</v>
       </c>
       <c r="H77" t="n">
-        <v>125.6270396270396</v>
+        <v>124.9215591136989</v>
       </c>
     </row>
     <row r="78">
@@ -2938,16 +2938,16 @@
         <v>9</v>
       </c>
       <c r="E78" t="n">
-        <v>110.1539015555555</v>
+        <v>109.1861615555555</v>
       </c>
       <c r="F78" t="n">
-        <v>125.4963306419378</v>
+        <v>124.3041998096129</v>
       </c>
       <c r="G78" t="n">
-        <v>125.8045727076505</v>
+        <v>124.6355701124575</v>
       </c>
       <c r="H78" t="n">
-        <v>106.2147094092253</v>
+        <v>104.8629213120573</v>
       </c>
     </row>
     <row r="79">
@@ -2970,16 +2970,16 @@
         <v>1</v>
       </c>
       <c r="E79" t="n">
-        <v>95.62525677777778</v>
+        <v>94.65034833333333</v>
       </c>
       <c r="F79" t="n">
-        <v>184.7869025134389</v>
+        <v>184.0377490003302</v>
       </c>
       <c r="G79" t="n">
-        <v>171.4039481330815</v>
+        <v>170.5397116548663</v>
       </c>
       <c r="H79" t="n">
-        <v>139.3933604532907</v>
+        <v>138.2357386551231</v>
       </c>
     </row>
     <row r="80">
@@ -3002,16 +3002,16 @@
         <v>2</v>
       </c>
       <c r="E80" t="n">
-        <v>60.2337505</v>
+        <v>59.60023922222222</v>
       </c>
       <c r="F80" t="n">
-        <v>173.4814087192673</v>
+        <v>172.7524813171415</v>
       </c>
       <c r="G80" t="n">
-        <v>160.9781873862422</v>
+        <v>160.1381071929005</v>
       </c>
       <c r="H80" t="n">
-        <v>120.5272874353567</v>
+        <v>119.2727113498365</v>
       </c>
     </row>
     <row r="81">
@@ -3034,16 +3034,16 @@
         <v>3</v>
       </c>
       <c r="E81" t="n">
-        <v>63.24808138888888</v>
+        <v>61.55722455555555</v>
       </c>
       <c r="F81" t="n">
-        <v>179.8612858045203</v>
+        <v>178.1708548382548</v>
       </c>
       <c r="G81" t="n">
-        <v>167.1140526734957</v>
+        <v>165.1539047296725</v>
       </c>
       <c r="H81" t="n">
-        <v>133.46104413259</v>
+        <v>130.6192853315283</v>
       </c>
     </row>
     <row r="82">
@@ -3066,16 +3066,16 @@
         <v>1</v>
       </c>
       <c r="E82" t="n">
-        <v>11.064494</v>
+        <v>10.96323972222222</v>
       </c>
       <c r="F82" t="n">
-        <v>154.2727415307403</v>
+        <v>153.4127888572333</v>
       </c>
       <c r="G82" t="n">
-        <v>154.1932245922208</v>
+        <v>153.3417220639443</v>
       </c>
       <c r="H82" t="n">
-        <v>132.0056461731493</v>
+        <v>130.9412788857233</v>
       </c>
     </row>
     <row r="83">
@@ -3098,16 +3098,16 @@
         <v>2</v>
       </c>
       <c r="E83" t="n">
-        <v>15.65409055555556</v>
+        <v>15.5402915</v>
       </c>
       <c r="F83" t="n">
-        <v>145.2431403292642</v>
+        <v>144.5463568689375</v>
       </c>
       <c r="G83" t="n">
-        <v>142.4632097659312</v>
+        <v>141.7558087074216</v>
       </c>
       <c r="H83" t="n">
-        <v>117.0264307313249</v>
+        <v>116.1304985337243</v>
       </c>
     </row>
     <row r="84">
@@ -3130,16 +3130,16 @@
         <v>3</v>
       </c>
       <c r="E84" t="n">
-        <v>6.486546166666666</v>
+        <v>6.368266833333333</v>
       </c>
       <c r="F84" t="n">
-        <v>157.7607296137339</v>
+        <v>156.1813712100519</v>
       </c>
       <c r="G84" t="n">
-        <v>158.0799356223176</v>
+        <v>156.5148866429937</v>
       </c>
       <c r="H84" t="n">
-        <v>139.9780042918455</v>
+        <v>138.0707456978967</v>
       </c>
     </row>
     <row r="85">
@@ -3162,16 +3162,16 @@
         <v>4</v>
       </c>
       <c r="E85" t="n">
-        <v>17.4112555</v>
+        <v>17.13347827777778</v>
       </c>
       <c r="F85" t="n">
-        <v>168.8328797500252</v>
+        <v>167.6437275985663</v>
       </c>
       <c r="G85" t="n">
-        <v>164.2415079125088</v>
+        <v>163.0008192524322</v>
       </c>
       <c r="H85" t="n">
-        <v>136.5579074690051</v>
+        <v>134.8571428571429</v>
       </c>
     </row>
     <row r="86">
@@ -3194,16 +3194,16 @@
         <v>5</v>
       </c>
       <c r="E86" t="n">
-        <v>11.76789761111111</v>
+        <v>11.59316677777778</v>
       </c>
       <c r="F86" t="n">
-        <v>160.0896755162242</v>
+        <v>158.8321605030693</v>
       </c>
       <c r="G86" t="n">
-        <v>160.6240412979351</v>
+        <v>159.4008085042671</v>
       </c>
       <c r="H86" t="n">
-        <v>134.0867256637168</v>
+        <v>132.4541098966911</v>
       </c>
     </row>
     <row r="87">
@@ -3226,16 +3226,16 @@
         <v>6</v>
       </c>
       <c r="E87" t="n">
-        <v>5.560024722222222</v>
+        <v>5.511637722222222</v>
       </c>
       <c r="F87" t="n">
-        <v>160.1744258224705</v>
+        <v>159.3850970569818</v>
       </c>
       <c r="G87" t="n">
-        <v>158.9338919925512</v>
+        <v>158.1386975579211</v>
       </c>
       <c r="H87" t="n">
-        <v>139.1436995654873</v>
+        <v>138.1728240450845</v>
       </c>
     </row>
     <row r="88">
@@ -3258,16 +3258,16 @@
         <v>7</v>
       </c>
       <c r="E88" t="n">
-        <v>17.04118455555555</v>
+        <v>16.94261844444444</v>
       </c>
       <c r="F88" t="n">
-        <v>160.1237644151565</v>
+        <v>159.6351491300746</v>
       </c>
       <c r="G88" t="n">
-        <v>157.0090609555189</v>
+        <v>156.5051781275891</v>
       </c>
       <c r="H88" t="n">
-        <v>121.1164538714992</v>
+        <v>120.3909486329743</v>
       </c>
     </row>
     <row r="89">
@@ -3290,16 +3290,16 @@
         <v>8</v>
       </c>
       <c r="E89" t="n">
-        <v>16.57344355555555</v>
+        <v>16.31179533333333</v>
       </c>
       <c r="F89" t="n">
-        <v>146.1279365079365</v>
+        <v>144.5994840374073</v>
       </c>
       <c r="G89" t="n">
-        <v>144.5933333333333</v>
+        <v>143.0657852305708</v>
       </c>
       <c r="H89" t="n">
-        <v>120.8440211640212</v>
+        <v>118.9223906266796</v>
       </c>
     </row>
     <row r="90">
@@ -3322,16 +3322,16 @@
         <v>9</v>
       </c>
       <c r="E90" t="n">
-        <v>5.117373277777777</v>
+        <v>5.072570499999999</v>
       </c>
       <c r="F90" t="n">
-        <v>147.8831870357866</v>
+        <v>147.0595846101464</v>
       </c>
       <c r="G90" t="n">
-        <v>150.0087778528022</v>
+        <v>149.2134831460674</v>
       </c>
       <c r="H90" t="n">
-        <v>131.1870357866307</v>
+        <v>130.2254000680967</v>
       </c>
     </row>
     <row r="91">
@@ -3354,16 +3354,16 @@
         <v>1</v>
       </c>
       <c r="E91" t="n">
-        <v>113.4388412222222</v>
+        <v>112.854613</v>
       </c>
       <c r="F91" t="n">
-        <v>142.7318001170708</v>
+        <v>142.2305667389284</v>
       </c>
       <c r="G91" t="n">
-        <v>140.8105610154349</v>
+        <v>140.2980644162279</v>
       </c>
       <c r="H91" t="n">
-        <v>117.0548076034382</v>
+        <v>116.4017497677299</v>
       </c>
     </row>
     <row r="92">
@@ -3386,16 +3386,16 @@
         <v>2</v>
       </c>
       <c r="E92" t="n">
-        <v>406.4758895555555</v>
+        <v>401.3504517777778</v>
       </c>
       <c r="F92" t="n">
-        <v>145.327171847883</v>
+        <v>144.3060410392639</v>
       </c>
       <c r="G92" t="n">
-        <v>144.9169735868328</v>
+        <v>143.9013251623028</v>
       </c>
       <c r="H92" t="n">
-        <v>126.1680999225306</v>
+        <v>124.8883190208791</v>
       </c>
     </row>
     <row r="93">
@@ -3418,16 +3418,16 @@
         <v>3</v>
       </c>
       <c r="E93" t="n">
-        <v>415.0108187222222</v>
+        <v>409.4534821666666</v>
       </c>
       <c r="F93" t="n">
-        <v>145.1317490186729</v>
+        <v>144.1141480001554</v>
       </c>
       <c r="G93" t="n">
-        <v>144.4489880197202</v>
+        <v>143.4405397358281</v>
       </c>
       <c r="H93" t="n">
-        <v>128.0630731503793</v>
+        <v>126.8060135581226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>